<commit_message>
question 2 in 12th
</commit_message>
<xml_diff>
--- a/automate/12th/res/example.xlsx
+++ b/automate/12th/res/example.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="96" windowWidth="9540" windowHeight="4512"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>Apples</t>
   </si>
@@ -39,25 +39,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -73,30 +76,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="22" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -386,121 +387,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="20.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>42099.565300925926</v>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="n">
+        <v>42099.56530092593</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="3" t="n">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>42099.153738425928</v>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="n">
+        <v>42099.15373842593</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="3" t="n">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>42100.532534722224</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s"/>
+      <c r="B3" s="2" t="s"/>
+      <c r="C3" s="3" t="s"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s"/>
+      <c r="B4" s="2" t="s"/>
+      <c r="C4" s="3" t="s"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="n">
+        <v>42100.53253472222</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C5" s="3" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>42102.374803240738</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="n">
+        <v>42102.37480324074</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C6" s="3" t="n">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>42104.088194444441</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="n">
+        <v>42104.08819444444</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C7" s="3" t="n">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>42104.757372685184</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="5" t="n">
+        <v>42104.75737268518</v>
+      </c>
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C8" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>42104.111643518518</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="5" t="n">
+        <v>42104.11164351852</v>
+      </c>
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C9" t="n">
         <v>98</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>